<commit_message>
Sprint 9 - Finalizada
</commit_message>
<xml_diff>
--- a/Sprint 9/Product Backlog-Burndown.xlsx
+++ b/Sprint 9/Product Backlog-Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="219">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -602,6 +602,87 @@
   </si>
   <si>
     <t>Codificação de métodos e parte gráfica</t>
+  </si>
+  <si>
+    <t>Divisão do sistema e suas funcionalidades para médico e atendente</t>
+  </si>
+  <si>
+    <t>Ajustes BD</t>
+  </si>
+  <si>
+    <t>Modificações e inclusões de funcionalidades</t>
+  </si>
+  <si>
+    <t>Melhoramento no código de busca e edição de prontuário</t>
+  </si>
+  <si>
+    <t>Melhoramento no controle de horários de agendamento</t>
+  </si>
+  <si>
+    <t>Separação de funcionalidades para cada usuário</t>
+  </si>
+  <si>
+    <t>Método de reconhecimento de tipo de usuário</t>
+  </si>
+  <si>
+    <t>Implementação gráfica com funcionalidades para cada tipo de usuário</t>
+  </si>
+  <si>
+    <t>Restrição de acesso para cada tipo de usuário</t>
+  </si>
+  <si>
+    <t>Criação de classe TelaMenuAtendente</t>
+  </si>
+  <si>
+    <t>Criação de classe TelaMenuMedico</t>
+  </si>
+  <si>
+    <t>Método de inserção de usuário padrão no banco de dados</t>
+  </si>
+  <si>
+    <t>Método de validação de acesso de usuário</t>
+  </si>
+  <si>
+    <t>Método de verificação de usuário padrão no banco</t>
+  </si>
+  <si>
+    <t>Método de busca de agendamentos do dia atual</t>
+  </si>
+  <si>
+    <t>Método de busca de agendamentos pelo cpf do funcionário</t>
+  </si>
+  <si>
+    <t>Método de busca de paciente por nome</t>
+  </si>
+  <si>
+    <t>Implementação de usuário default no banco</t>
+  </si>
+  <si>
+    <t>Inclusão de JRadioButton e ButtonGroup na tela de cadastro de funcionário</t>
+  </si>
+  <si>
+    <t>Inserção de tabela com todas as consultas do dia na TelaMenuAtendente</t>
+  </si>
+  <si>
+    <t>Inserção de tabela com todos os pacientes do dia na TelaMenuMedico</t>
+  </si>
+  <si>
+    <t>Inserção de JMenu Opções na TelaMenuAtendende</t>
+  </si>
+  <si>
+    <t>Inserção de JMenu Opções na TelaMenuMédico</t>
+  </si>
+  <si>
+    <t>Inserção de JMenuItem Sair na TelaMenuAtendende</t>
+  </si>
+  <si>
+    <t>Inserção de JMenuItem Sair na TelaMenuMedico</t>
+  </si>
+  <si>
+    <t>Implementação de método de encerramento do sistema</t>
+  </si>
+  <si>
+    <t>Restrição de funções para cada tipo de usuário</t>
   </si>
 </sst>
 </file>
@@ -916,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1049,24 +1130,51 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1082,33 +1190,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1132,6 +1213,42 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1372,7 +1489,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
+                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1499,10 +1616,10 @@
                   <c:v>226.51999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>226.51999999999998</c:v>
+                  <c:v>183.26999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>226.51999999999998</c:v>
+                  <c:v>183.26999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1516,7 +1633,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
+                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1582,11 +1699,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="245197920"/>
-        <c:axId val="245198312"/>
+        <c:axId val="232819040"/>
+        <c:axId val="232819432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="245197920"/>
+        <c:axId val="232819040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1738,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245198312"/>
+        <c:crossAx val="232819432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1746,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245198312"/>
+        <c:axId val="232819432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1675,7 +1792,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245197920"/>
+        <c:crossAx val="232819040"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2056,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S137"/>
+  <dimension ref="A1:S163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2074,14 +2191,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2285,10 +2402,10 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="67" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -2318,8 +2435,8 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="57"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="23" t="s">
         <v>43</v>
       </c>
@@ -2347,8 +2464,8 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="23" t="s">
         <v>44</v>
       </c>
@@ -2376,8 +2493,8 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="23" t="s">
         <v>45</v>
       </c>
@@ -2405,8 +2522,8 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="23" t="s">
         <v>46</v>
       </c>
@@ -2434,8 +2551,8 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
-      <c r="B13" s="59"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="23" t="s">
         <v>47</v>
       </c>
@@ -2463,8 +2580,8 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
-      <c r="B14" s="60"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="23" t="s">
         <v>48</v>
       </c>
@@ -2492,10 +2609,10 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="53" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -2525,8 +2642,8 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="54"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="24" t="s">
         <v>52</v>
       </c>
@@ -2554,8 +2671,8 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="24" t="s">
         <v>54</v>
       </c>
@@ -2583,8 +2700,8 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="55"/>
-      <c r="B18" s="51"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="25" t="s">
         <v>53</v>
       </c>
@@ -2612,10 +2729,10 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="53" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="22" t="s">
@@ -2645,8 +2762,8 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="55"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="23" t="s">
         <v>73</v>
       </c>
@@ -2674,10 +2791,10 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="53" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="22" t="s">
@@ -2707,8 +2824,8 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="55"/>
-      <c r="B22" s="51"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="23" t="s">
         <v>73</v>
       </c>
@@ -2736,10 +2853,10 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="53" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="22" t="s">
@@ -2769,8 +2886,8 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55"/>
-      <c r="B24" s="51"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="23" t="s">
         <v>73</v>
       </c>
@@ -2798,10 +2915,10 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="53" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="22" t="s">
@@ -2831,8 +2948,8 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="55"/>
-      <c r="B26" s="51"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="23" t="s">
         <v>73</v>
       </c>
@@ -2860,10 +2977,10 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="59" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="22" t="s">
@@ -2893,8 +3010,8 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="55"/>
-      <c r="B28" s="62"/>
+      <c r="A28" s="63"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="22" t="s">
         <v>75</v>
       </c>
@@ -2922,10 +3039,10 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="53" t="s">
         <v>89</v>
       </c>
       <c r="C29" s="33" t="s">
@@ -2955,8 +3072,8 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="38" t="s">
         <v>81</v>
       </c>
@@ -2984,10 +3101,10 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="53" t="s">
         <v>90</v>
       </c>
       <c r="C31" s="39" t="s">
@@ -3017,8 +3134,8 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="52"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="40" t="s">
         <v>83</v>
       </c>
@@ -3046,8 +3163,8 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="52"/>
-      <c r="B33" s="52"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="41" t="s">
         <v>84</v>
       </c>
@@ -3075,8 +3192,8 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="42" t="s">
         <v>85</v>
       </c>
@@ -3104,8 +3221,8 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="42" t="s">
         <v>86</v>
       </c>
@@ -3133,10 +3250,10 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="53" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="39" t="s">
@@ -3166,8 +3283,8 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="51"/>
-      <c r="B37" s="51"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="55"/>
       <c r="C37" s="39" t="s">
         <v>88</v>
       </c>
@@ -3195,10 +3312,10 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="50"/>
+      <c r="B38" s="53"/>
       <c r="C38" s="33" t="s">
         <v>96</v>
       </c>
@@ -3226,8 +3343,8 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="64"/>
-      <c r="B39" s="52"/>
+      <c r="A39" s="57"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="38" t="s">
         <v>97</v>
       </c>
@@ -3255,8 +3372,8 @@
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="65"/>
-      <c r="B40" s="51"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="39" t="s">
         <v>98</v>
       </c>
@@ -3284,10 +3401,10 @@
       <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="53" t="s">
         <v>106</v>
       </c>
       <c r="C41" s="39" t="s">
@@ -3317,8 +3434,8 @@
       <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="67"/>
-      <c r="B42" s="52"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="39" t="s">
         <v>100</v>
       </c>
@@ -3346,8 +3463,8 @@
       <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="67"/>
-      <c r="B43" s="52"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="41" t="s">
         <v>101</v>
       </c>
@@ -3375,8 +3492,8 @@
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="67"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="42" t="s">
         <v>101</v>
       </c>
@@ -3404,8 +3521,8 @@
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="68"/>
-      <c r="B45" s="51"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="41" t="s">
         <v>109</v>
       </c>
@@ -3433,10 +3550,10 @@
       <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="53" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="42" t="s">
@@ -3466,8 +3583,8 @@
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="68"/>
-      <c r="B47" s="51"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="42" t="s">
         <v>103</v>
       </c>
@@ -3495,10 +3612,10 @@
       <c r="S47" s="1"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="53" t="s">
         <v>108</v>
       </c>
       <c r="C48" s="39" t="s">
@@ -3528,8 +3645,8 @@
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="68"/>
-      <c r="B49" s="51"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="39" t="s">
         <v>105</v>
       </c>
@@ -3557,10 +3674,10 @@
       <c r="S49" s="1"/>
     </row>
     <row r="50" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="63" t="s">
+      <c r="A50" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="59" t="s">
         <v>138</v>
       </c>
       <c r="C50" s="33" t="s">
@@ -3590,8 +3707,8 @@
       <c r="S50" s="1"/>
     </row>
     <row r="51" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="64"/>
-      <c r="B51" s="69"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="60"/>
       <c r="C51" s="38" t="s">
         <v>117</v>
       </c>
@@ -3619,8 +3736,8 @@
       <c r="S51" s="1"/>
     </row>
     <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="65"/>
-      <c r="B52" s="62"/>
+      <c r="A52" s="58"/>
+      <c r="B52" s="61"/>
       <c r="C52" s="39" t="s">
         <v>144</v>
       </c>
@@ -3648,10 +3765,10 @@
       <c r="S52" s="1"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="53" t="s">
         <v>139</v>
       </c>
       <c r="C53" s="39" t="s">
@@ -3681,8 +3798,8 @@
       <c r="S53" s="1"/>
     </row>
     <row r="54" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="67"/>
-      <c r="B54" s="52"/>
+      <c r="A54" s="51"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="39" t="s">
         <v>119</v>
       </c>
@@ -3710,8 +3827,8 @@
       <c r="S54" s="1"/>
     </row>
     <row r="55" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="67"/>
-      <c r="B55" s="52"/>
+      <c r="A55" s="51"/>
+      <c r="B55" s="54"/>
       <c r="C55" s="41" t="s">
         <v>120</v>
       </c>
@@ -3739,8 +3856,8 @@
       <c r="S55" s="1"/>
     </row>
     <row r="56" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="67"/>
-      <c r="B56" s="52"/>
+      <c r="A56" s="51"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="42" t="s">
         <v>121</v>
       </c>
@@ -3768,8 +3885,8 @@
       <c r="S56" s="1"/>
     </row>
     <row r="57" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="68"/>
-      <c r="B57" s="51"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="41" t="s">
         <v>122</v>
       </c>
@@ -3797,10 +3914,10 @@
       <c r="S57" s="1"/>
     </row>
     <row r="58" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="53" t="s">
         <v>140</v>
       </c>
       <c r="C58" s="42" t="s">
@@ -3830,8 +3947,8 @@
       <c r="S58" s="1"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="68"/>
-      <c r="B59" s="51"/>
+      <c r="A59" s="52"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="42" t="s">
         <v>124</v>
       </c>
@@ -3859,10 +3976,10 @@
       <c r="S59" s="1"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="61" t="s">
+      <c r="B60" s="59" t="s">
         <v>141</v>
       </c>
       <c r="C60" s="46" t="s">
@@ -3892,8 +4009,8 @@
       <c r="S60" s="1"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="67"/>
-      <c r="B61" s="69"/>
+      <c r="A61" s="51"/>
+      <c r="B61" s="60"/>
       <c r="C61" s="42" t="s">
         <v>126</v>
       </c>
@@ -3921,8 +4038,8 @@
       <c r="S61" s="1"/>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="67"/>
-      <c r="B62" s="69"/>
+      <c r="A62" s="51"/>
+      <c r="B62" s="60"/>
       <c r="C62" s="39" t="s">
         <v>127</v>
       </c>
@@ -3950,8 +4067,8 @@
       <c r="S62" s="1"/>
     </row>
     <row r="63" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="67"/>
-      <c r="B63" s="69"/>
+      <c r="A63" s="51"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="39" t="s">
         <v>128</v>
       </c>
@@ -3979,8 +4096,8 @@
       <c r="S63" s="1"/>
     </row>
     <row r="64" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="67"/>
-      <c r="B64" s="69"/>
+      <c r="A64" s="51"/>
+      <c r="B64" s="60"/>
       <c r="C64" s="39" t="s">
         <v>129</v>
       </c>
@@ -4008,8 +4125,8 @@
       <c r="S64" s="1"/>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="67"/>
-      <c r="B65" s="69"/>
+      <c r="A65" s="51"/>
+      <c r="B65" s="60"/>
       <c r="C65" s="39" t="s">
         <v>130</v>
       </c>
@@ -4037,8 +4154,8 @@
       <c r="S65" s="1"/>
     </row>
     <row r="66" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="67"/>
-      <c r="B66" s="69"/>
+      <c r="A66" s="51"/>
+      <c r="B66" s="60"/>
       <c r="C66" s="39" t="s">
         <v>131</v>
       </c>
@@ -4066,8 +4183,8 @@
       <c r="S66" s="1"/>
     </row>
     <row r="67" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="67"/>
-      <c r="B67" s="69"/>
+      <c r="A67" s="51"/>
+      <c r="B67" s="60"/>
       <c r="C67" s="39" t="s">
         <v>132</v>
       </c>
@@ -4095,8 +4212,8 @@
       <c r="S67" s="1"/>
     </row>
     <row r="68" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="67"/>
-      <c r="B68" s="69"/>
+      <c r="A68" s="51"/>
+      <c r="B68" s="60"/>
       <c r="C68" s="39" t="s">
         <v>133</v>
       </c>
@@ -4124,8 +4241,8 @@
       <c r="S68" s="1"/>
     </row>
     <row r="69" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="67"/>
-      <c r="B69" s="62"/>
+      <c r="A69" s="51"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="39" t="s">
         <v>134</v>
       </c>
@@ -4153,10 +4270,10 @@
       <c r="S69" s="1"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="66" t="s">
+      <c r="A70" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="B70" s="53" t="s">
         <v>142</v>
       </c>
       <c r="C70" s="47" t="s">
@@ -4186,8 +4303,8 @@
       <c r="S70" s="1"/>
     </row>
     <row r="71" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="67"/>
-      <c r="B71" s="52"/>
+      <c r="A71" s="51"/>
+      <c r="B71" s="54"/>
       <c r="C71" s="39" t="s">
         <v>136</v>
       </c>
@@ -4215,8 +4332,8 @@
       <c r="S71" s="1"/>
     </row>
     <row r="72" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="68"/>
-      <c r="B72" s="51"/>
+      <c r="A72" s="52"/>
+      <c r="B72" s="55"/>
       <c r="C72" s="39" t="s">
         <v>137</v>
       </c>
@@ -4244,10 +4361,10 @@
       <c r="S72" s="1"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="66" t="s">
+      <c r="A73" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="B73" s="50" t="s">
+      <c r="B73" s="53" t="s">
         <v>143</v>
       </c>
       <c r="C73" s="33" t="s">
@@ -4277,8 +4394,8 @@
       <c r="S73" s="1"/>
     </row>
     <row r="74" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="67"/>
-      <c r="B74" s="52"/>
+      <c r="A74" s="51"/>
+      <c r="B74" s="54"/>
       <c r="C74" s="38" t="s">
         <v>97</v>
       </c>
@@ -4306,8 +4423,8 @@
       <c r="S74" s="1"/>
     </row>
     <row r="75" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="68"/>
-      <c r="B75" s="51"/>
+      <c r="A75" s="52"/>
+      <c r="B75" s="55"/>
       <c r="C75" s="39" t="s">
         <v>98</v>
       </c>
@@ -4335,10 +4452,10 @@
       <c r="S75" s="1"/>
     </row>
     <row r="76" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="63" t="s">
+      <c r="A76" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="50" t="s">
+      <c r="B76" s="53" t="s">
         <v>188</v>
       </c>
       <c r="C76" s="33" t="s">
@@ -4368,8 +4485,8 @@
       <c r="S76" s="1"/>
     </row>
     <row r="77" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="64"/>
-      <c r="B77" s="52"/>
+      <c r="A77" s="57"/>
+      <c r="B77" s="54"/>
       <c r="C77" s="38" t="s">
         <v>148</v>
       </c>
@@ -4397,8 +4514,8 @@
       <c r="S77" s="1"/>
     </row>
     <row r="78" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="65"/>
-      <c r="B78" s="51"/>
+      <c r="A78" s="58"/>
+      <c r="B78" s="55"/>
       <c r="C78" s="39" t="s">
         <v>149</v>
       </c>
@@ -4426,10 +4543,10 @@
       <c r="S78" s="1"/>
     </row>
     <row r="79" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="66" t="s">
+      <c r="A79" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="50" t="s">
+      <c r="B79" s="53" t="s">
         <v>189</v>
       </c>
       <c r="C79" s="39" t="s">
@@ -4459,8 +4576,8 @@
       <c r="S79" s="1"/>
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="67"/>
-      <c r="B80" s="52"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="54"/>
       <c r="C80" s="39" t="s">
         <v>151</v>
       </c>
@@ -4488,8 +4605,8 @@
       <c r="S80" s="1"/>
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="67"/>
-      <c r="B81" s="52"/>
+      <c r="A81" s="51"/>
+      <c r="B81" s="54"/>
       <c r="C81" s="41" t="s">
         <v>152</v>
       </c>
@@ -4517,8 +4634,8 @@
       <c r="S81" s="1"/>
     </row>
     <row r="82" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="67"/>
-      <c r="B82" s="52"/>
+      <c r="A82" s="51"/>
+      <c r="B82" s="54"/>
       <c r="C82" s="42" t="s">
         <v>153</v>
       </c>
@@ -4546,8 +4663,8 @@
       <c r="S82" s="1"/>
     </row>
     <row r="83" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="68"/>
-      <c r="B83" s="51"/>
+      <c r="A83" s="52"/>
+      <c r="B83" s="55"/>
       <c r="C83" s="41" t="s">
         <v>154</v>
       </c>
@@ -4575,10 +4692,10 @@
       <c r="S83" s="1"/>
     </row>
     <row r="84" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="66" t="s">
+      <c r="A84" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="50" t="s">
+      <c r="B84" s="53" t="s">
         <v>190</v>
       </c>
       <c r="C84" s="42" t="s">
@@ -4608,8 +4725,8 @@
       <c r="S84" s="1"/>
     </row>
     <row r="85" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="67"/>
-      <c r="B85" s="52"/>
+      <c r="A85" s="51"/>
+      <c r="B85" s="54"/>
       <c r="C85" s="42" t="s">
         <v>156</v>
       </c>
@@ -4637,8 +4754,8 @@
       <c r="S85" s="1"/>
     </row>
     <row r="86" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="67"/>
-      <c r="B86" s="52"/>
+      <c r="A86" s="51"/>
+      <c r="B86" s="54"/>
       <c r="C86" s="42" t="s">
         <v>157</v>
       </c>
@@ -4666,8 +4783,8 @@
       <c r="S86" s="1"/>
     </row>
     <row r="87" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="67"/>
-      <c r="B87" s="52"/>
+      <c r="A87" s="51"/>
+      <c r="B87" s="54"/>
       <c r="C87" s="42" t="s">
         <v>158</v>
       </c>
@@ -4695,8 +4812,8 @@
       <c r="S87" s="1"/>
     </row>
     <row r="88" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="67"/>
-      <c r="B88" s="52"/>
+      <c r="A88" s="51"/>
+      <c r="B88" s="54"/>
       <c r="C88" s="42" t="s">
         <v>159</v>
       </c>
@@ -4724,8 +4841,8 @@
       <c r="S88" s="1"/>
     </row>
     <row r="89" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="67"/>
-      <c r="B89" s="52"/>
+      <c r="A89" s="51"/>
+      <c r="B89" s="54"/>
       <c r="C89" s="42" t="s">
         <v>160</v>
       </c>
@@ -4753,8 +4870,8 @@
       <c r="S89" s="1"/>
     </row>
     <row r="90" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="67"/>
-      <c r="B90" s="52"/>
+      <c r="A90" s="51"/>
+      <c r="B90" s="54"/>
       <c r="C90" s="42" t="s">
         <v>161</v>
       </c>
@@ -4782,8 +4899,8 @@
       <c r="S90" s="1"/>
     </row>
     <row r="91" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="67"/>
-      <c r="B91" s="52"/>
+      <c r="A91" s="51"/>
+      <c r="B91" s="54"/>
       <c r="C91" s="42" t="s">
         <v>162</v>
       </c>
@@ -4811,8 +4928,8 @@
       <c r="S91" s="1"/>
     </row>
     <row r="92" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="67"/>
-      <c r="B92" s="52"/>
+      <c r="A92" s="51"/>
+      <c r="B92" s="54"/>
       <c r="C92" s="42" t="s">
         <v>163</v>
       </c>
@@ -4840,8 +4957,8 @@
       <c r="S92" s="1"/>
     </row>
     <row r="93" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="67"/>
-      <c r="B93" s="52"/>
+      <c r="A93" s="51"/>
+      <c r="B93" s="54"/>
       <c r="C93" s="42" t="s">
         <v>164</v>
       </c>
@@ -4869,8 +4986,8 @@
       <c r="S93" s="1"/>
     </row>
     <row r="94" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="67"/>
-      <c r="B94" s="52"/>
+      <c r="A94" s="51"/>
+      <c r="B94" s="54"/>
       <c r="C94" s="42" t="s">
         <v>165</v>
       </c>
@@ -4898,8 +5015,8 @@
       <c r="S94" s="1"/>
     </row>
     <row r="95" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="67"/>
-      <c r="B95" s="52"/>
+      <c r="A95" s="51"/>
+      <c r="B95" s="54"/>
       <c r="C95" s="42" t="s">
         <v>166</v>
       </c>
@@ -4927,8 +5044,8 @@
       <c r="S95" s="1"/>
     </row>
     <row r="96" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="67"/>
-      <c r="B96" s="52"/>
+      <c r="A96" s="51"/>
+      <c r="B96" s="54"/>
       <c r="C96" s="42" t="s">
         <v>167</v>
       </c>
@@ -4956,8 +5073,8 @@
       <c r="S96" s="1"/>
     </row>
     <row r="97" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="67"/>
-      <c r="B97" s="52"/>
+      <c r="A97" s="51"/>
+      <c r="B97" s="54"/>
       <c r="C97" s="42" t="s">
         <v>168</v>
       </c>
@@ -4985,8 +5102,8 @@
       <c r="S97" s="1"/>
     </row>
     <row r="98" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="67"/>
-      <c r="B98" s="52"/>
+      <c r="A98" s="51"/>
+      <c r="B98" s="54"/>
       <c r="C98" s="42" t="s">
         <v>169</v>
       </c>
@@ -5014,8 +5131,8 @@
       <c r="S98" s="1"/>
     </row>
     <row r="99" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="67"/>
-      <c r="B99" s="52"/>
+      <c r="A99" s="51"/>
+      <c r="B99" s="54"/>
       <c r="C99" s="42" t="s">
         <v>170</v>
       </c>
@@ -5043,8 +5160,8 @@
       <c r="S99" s="1"/>
     </row>
     <row r="100" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="67"/>
-      <c r="B100" s="52"/>
+      <c r="A100" s="51"/>
+      <c r="B100" s="54"/>
       <c r="C100" s="42" t="s">
         <v>171</v>
       </c>
@@ -5072,8 +5189,8 @@
       <c r="S100" s="1"/>
     </row>
     <row r="101" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="67"/>
-      <c r="B101" s="52"/>
+      <c r="A101" s="51"/>
+      <c r="B101" s="54"/>
       <c r="C101" s="42" t="s">
         <v>172</v>
       </c>
@@ -5101,8 +5218,8 @@
       <c r="S101" s="1"/>
     </row>
     <row r="102" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="67"/>
-      <c r="B102" s="52"/>
+      <c r="A102" s="51"/>
+      <c r="B102" s="54"/>
       <c r="C102" s="42" t="s">
         <v>173</v>
       </c>
@@ -5130,8 +5247,8 @@
       <c r="S102" s="1"/>
     </row>
     <row r="103" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="67"/>
-      <c r="B103" s="52"/>
+      <c r="A103" s="51"/>
+      <c r="B103" s="54"/>
       <c r="C103" s="42" t="s">
         <v>174</v>
       </c>
@@ -5159,8 +5276,8 @@
       <c r="S103" s="1"/>
     </row>
     <row r="104" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="67"/>
-      <c r="B104" s="52"/>
+      <c r="A104" s="51"/>
+      <c r="B104" s="54"/>
       <c r="C104" s="39" t="s">
         <v>175</v>
       </c>
@@ -5188,8 +5305,8 @@
       <c r="S104" s="1"/>
     </row>
     <row r="105" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="67"/>
-      <c r="B105" s="52"/>
+      <c r="A105" s="51"/>
+      <c r="B105" s="54"/>
       <c r="C105" s="39" t="s">
         <v>176</v>
       </c>
@@ -5217,8 +5334,8 @@
       <c r="S105" s="1"/>
     </row>
     <row r="106" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="67"/>
-      <c r="B106" s="52"/>
+      <c r="A106" s="51"/>
+      <c r="B106" s="54"/>
       <c r="C106" s="39" t="s">
         <v>177</v>
       </c>
@@ -5246,8 +5363,8 @@
       <c r="S106" s="1"/>
     </row>
     <row r="107" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="67"/>
-      <c r="B107" s="52"/>
+      <c r="A107" s="51"/>
+      <c r="B107" s="54"/>
       <c r="C107" s="39" t="s">
         <v>178</v>
       </c>
@@ -5275,8 +5392,8 @@
       <c r="S107" s="1"/>
     </row>
     <row r="108" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="67"/>
-      <c r="B108" s="52"/>
+      <c r="A108" s="51"/>
+      <c r="B108" s="54"/>
       <c r="C108" s="39" t="s">
         <v>179</v>
       </c>
@@ -5304,8 +5421,8 @@
       <c r="S108" s="1"/>
     </row>
     <row r="109" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="67"/>
-      <c r="B109" s="52"/>
+      <c r="A109" s="51"/>
+      <c r="B109" s="54"/>
       <c r="C109" s="39" t="s">
         <v>180</v>
       </c>
@@ -5333,8 +5450,8 @@
       <c r="S109" s="1"/>
     </row>
     <row r="110" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="67"/>
-      <c r="B110" s="52"/>
+      <c r="A110" s="51"/>
+      <c r="B110" s="54"/>
       <c r="C110" s="39" t="s">
         <v>181</v>
       </c>
@@ -5362,8 +5479,8 @@
       <c r="S110" s="1"/>
     </row>
     <row r="111" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="67"/>
-      <c r="B111" s="52"/>
+      <c r="A111" s="51"/>
+      <c r="B111" s="54"/>
       <c r="C111" s="39" t="s">
         <v>182</v>
       </c>
@@ -5391,8 +5508,8 @@
       <c r="S111" s="1"/>
     </row>
     <row r="112" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="67"/>
-      <c r="B112" s="52"/>
+      <c r="A112" s="51"/>
+      <c r="B112" s="54"/>
       <c r="C112" s="39" t="s">
         <v>183</v>
       </c>
@@ -5420,8 +5537,8 @@
       <c r="S112" s="1"/>
     </row>
     <row r="113" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="68"/>
-      <c r="B113" s="51"/>
+      <c r="A113" s="52"/>
+      <c r="B113" s="55"/>
       <c r="C113" s="39" t="s">
         <v>184</v>
       </c>
@@ -5449,10 +5566,10 @@
       <c r="S113" s="1"/>
     </row>
     <row r="114" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="66" t="s">
+      <c r="A114" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B114" s="50" t="s">
+      <c r="B114" s="53" t="s">
         <v>191</v>
       </c>
       <c r="C114" s="39" t="s">
@@ -5482,8 +5599,8 @@
       <c r="S114" s="1"/>
     </row>
     <row r="115" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="67"/>
-      <c r="B115" s="52"/>
+      <c r="A115" s="51"/>
+      <c r="B115" s="54"/>
       <c r="C115" s="39" t="s">
         <v>185</v>
       </c>
@@ -5511,8 +5628,8 @@
       <c r="S115" s="1"/>
     </row>
     <row r="116" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="68"/>
-      <c r="B116" s="51"/>
+      <c r="A116" s="52"/>
+      <c r="B116" s="55"/>
       <c r="C116" s="39" t="s">
         <v>186</v>
       </c>
@@ -5540,10 +5657,10 @@
       <c r="S116" s="1"/>
     </row>
     <row r="117" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="66" t="s">
+      <c r="A117" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="B117" s="50" t="s">
+      <c r="B117" s="53" t="s">
         <v>143</v>
       </c>
       <c r="C117" s="33" t="s">
@@ -5573,8 +5690,8 @@
       <c r="S117" s="1"/>
     </row>
     <row r="118" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="67"/>
-      <c r="B118" s="52"/>
+      <c r="A118" s="51"/>
+      <c r="B118" s="54"/>
       <c r="C118" s="38" t="s">
         <v>97</v>
       </c>
@@ -5602,8 +5719,8 @@
       <c r="S118" s="1"/>
     </row>
     <row r="119" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="67"/>
-      <c r="B119" s="52"/>
+      <c r="A119" s="51"/>
+      <c r="B119" s="54"/>
       <c r="C119" s="39" t="s">
         <v>98</v>
       </c>
@@ -5631,8 +5748,8 @@
       <c r="S119" s="1"/>
     </row>
     <row r="120" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="67"/>
-      <c r="B120" s="51"/>
+      <c r="A120" s="51"/>
+      <c r="B120" s="55"/>
       <c r="C120" s="39" t="s">
         <v>187</v>
       </c>
@@ -5659,13 +5776,25 @@
       <c r="R120" s="1"/>
       <c r="S120" s="1"/>
     </row>
-    <row r="121" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A121" s="48"/>
-      <c r="B121" s="49"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="35"/>
-      <c r="E121" s="35"/>
-      <c r="F121" s="6"/>
+    <row r="121" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B121" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="C121" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D121" s="85">
+        <v>1</v>
+      </c>
+      <c r="E121" s="85">
+        <v>1</v>
+      </c>
+      <c r="F121" s="6">
+        <v>9</v>
+      </c>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
@@ -5680,13 +5809,21 @@
       <c r="R121" s="1"/>
       <c r="S121" s="1"/>
     </row>
-    <row r="122" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A122" s="48"/>
-      <c r="B122" s="49"/>
-      <c r="C122" s="39"/>
-      <c r="D122" s="35"/>
-      <c r="E122" s="35"/>
-      <c r="F122" s="6"/>
+    <row r="122" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="80"/>
+      <c r="B122" s="54"/>
+      <c r="C122" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="D122" s="85">
+        <v>0.5</v>
+      </c>
+      <c r="E122" s="85">
+        <v>0.75</v>
+      </c>
+      <c r="F122" s="6">
+        <v>9</v>
+      </c>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
@@ -5701,13 +5838,21 @@
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
     </row>
-    <row r="123" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A123" s="48"/>
-      <c r="B123" s="49"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="35"/>
-      <c r="E123" s="35"/>
-      <c r="F123" s="6"/>
+    <row r="123" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="80"/>
+      <c r="B123" s="54"/>
+      <c r="C123" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="D123" s="85">
+        <v>2</v>
+      </c>
+      <c r="E123" s="85">
+        <v>1.5</v>
+      </c>
+      <c r="F123" s="6">
+        <v>9</v>
+      </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
@@ -5722,13 +5867,21 @@
       <c r="R123" s="1"/>
       <c r="S123" s="1"/>
     </row>
-    <row r="124" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A124" s="48"/>
-      <c r="B124" s="49"/>
-      <c r="C124" s="39"/>
-      <c r="D124" s="35"/>
-      <c r="E124" s="35"/>
-      <c r="F124" s="6"/>
+    <row r="124" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="80"/>
+      <c r="B124" s="54"/>
+      <c r="C124" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="D124" s="85">
+        <v>1.5</v>
+      </c>
+      <c r="E124" s="85">
+        <v>2</v>
+      </c>
+      <c r="F124" s="6">
+        <v>9</v>
+      </c>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
@@ -5743,13 +5896,21 @@
       <c r="R124" s="1"/>
       <c r="S124" s="1"/>
     </row>
-    <row r="125" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A125" s="48"/>
-      <c r="B125" s="49"/>
-      <c r="C125" s="39"/>
-      <c r="D125" s="35"/>
-      <c r="E125" s="35"/>
-      <c r="F125" s="6"/>
+    <row r="125" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="81"/>
+      <c r="B125" s="55"/>
+      <c r="C125" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D125" s="86">
+        <v>3</v>
+      </c>
+      <c r="E125" s="86">
+        <v>3</v>
+      </c>
+      <c r="F125" s="6">
+        <v>9</v>
+      </c>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
@@ -5764,13 +5925,25 @@
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
     </row>
-    <row r="126" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A126" s="48"/>
-      <c r="B126" s="49"/>
-      <c r="C126" s="39"/>
-      <c r="D126" s="35"/>
-      <c r="E126" s="35"/>
-      <c r="F126" s="6"/>
+    <row r="126" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="82" t="s">
+        <v>192</v>
+      </c>
+      <c r="B126" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="C126" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="D126" s="89">
+        <v>2.75</v>
+      </c>
+      <c r="E126" s="87">
+        <v>3</v>
+      </c>
+      <c r="F126" s="6">
+        <v>9</v>
+      </c>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
@@ -5785,13 +5958,21 @@
       <c r="R126" s="1"/>
       <c r="S126" s="1"/>
     </row>
-    <row r="127" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A127" s="48"/>
-      <c r="B127" s="37"/>
-      <c r="C127" s="39"/>
-      <c r="D127" s="35"/>
-      <c r="E127" s="35"/>
-      <c r="F127" s="6"/>
+    <row r="127" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="83"/>
+      <c r="B127" s="54"/>
+      <c r="C127" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="D127" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="E127" s="88">
+        <v>1</v>
+      </c>
+      <c r="F127" s="6">
+        <v>9</v>
+      </c>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
@@ -5806,13 +5987,21 @@
       <c r="R127" s="1"/>
       <c r="S127" s="1"/>
     </row>
-    <row r="128" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A128" s="48"/>
-      <c r="B128" s="37"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="35"/>
-      <c r="E128" s="35"/>
-      <c r="F128" s="6"/>
+    <row r="128" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="83"/>
+      <c r="B128" s="54"/>
+      <c r="C128" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="D128" s="88">
+        <v>2</v>
+      </c>
+      <c r="E128" s="88">
+        <v>2.5</v>
+      </c>
+      <c r="F128" s="6">
+        <v>9</v>
+      </c>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
@@ -5827,13 +6016,21 @@
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
     </row>
-    <row r="129" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="45"/>
-      <c r="B129" s="4"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="28"/>
-      <c r="E129" s="5"/>
-      <c r="F129" s="6"/>
+    <row r="129" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="83"/>
+      <c r="B129" s="54"/>
+      <c r="C129" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="D129" s="88">
+        <v>2.25</v>
+      </c>
+      <c r="E129" s="88">
+        <v>2.25</v>
+      </c>
+      <c r="F129" s="6">
+        <v>9</v>
+      </c>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
@@ -5848,15 +6045,21 @@
       <c r="R129" s="1"/>
       <c r="S129" s="1"/>
     </row>
-    <row r="130" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="36"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="9"/>
+    <row r="130" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="83"/>
+      <c r="B130" s="54"/>
+      <c r="C130" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="D130" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E130" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F130" s="6">
+        <v>9</v>
+      </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
@@ -5871,13 +6074,21 @@
       <c r="R130" s="1"/>
       <c r="S130" s="1"/>
     </row>
-    <row r="131" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A131" s="7"/>
-      <c r="B131" s="4"/>
-      <c r="C131" s="4"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="6"/>
+    <row r="131" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="84"/>
+      <c r="B131" s="55"/>
+      <c r="C131" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="D131" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E131" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F131" s="6">
+        <v>9</v>
+      </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
@@ -5892,13 +6103,25 @@
       <c r="R131" s="1"/>
       <c r="S131" s="1"/>
     </row>
-    <row r="132" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="6"/>
+    <row r="132" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="82" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C132" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="D132" s="88">
+        <v>2</v>
+      </c>
+      <c r="E132" s="88">
+        <v>2.25</v>
+      </c>
+      <c r="F132" s="6">
+        <v>9</v>
+      </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
@@ -5913,15 +6136,21 @@
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
     </row>
-    <row r="133" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
+    <row r="133" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="83"/>
+      <c r="B133" s="54"/>
+      <c r="C133" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="D133" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="E133" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="F133" s="6">
         <v>9</v>
       </c>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
-      <c r="F133" s="9"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
@@ -5936,13 +6165,21 @@
       <c r="R133" s="1"/>
       <c r="S133" s="1"/>
     </row>
-    <row r="134" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="6"/>
+    <row r="134" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="83"/>
+      <c r="B134" s="54"/>
+      <c r="C134" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="D134" s="88">
+        <v>2.25</v>
+      </c>
+      <c r="E134" s="88">
+        <v>2</v>
+      </c>
+      <c r="F134" s="6">
+        <v>9</v>
+      </c>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
@@ -5957,13 +6194,21 @@
       <c r="R134" s="1"/>
       <c r="S134" s="1"/>
     </row>
-    <row r="135" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="5"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="6"/>
+    <row r="135" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="83"/>
+      <c r="B135" s="54"/>
+      <c r="C135" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="D135" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="E135" s="88">
+        <v>2</v>
+      </c>
+      <c r="F135" s="6">
+        <v>9</v>
+      </c>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
@@ -5978,21 +6223,21 @@
       <c r="R135" s="1"/>
       <c r="S135" s="1"/>
     </row>
-    <row r="136" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A136" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B136" s="4"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="11">
-        <f>SUM(D4:D135)</f>
-        <v>276.39999999999975</v>
-      </c>
-      <c r="E136" s="11">
-        <f>SUM(E4:E135)</f>
-        <v>273.47999999999996</v>
-      </c>
-      <c r="F136" s="6"/>
+    <row r="136" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="83"/>
+      <c r="B136" s="54"/>
+      <c r="C136" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D136" s="88">
+        <v>1.25</v>
+      </c>
+      <c r="E136" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="F136" s="6">
+        <v>9</v>
+      </c>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
@@ -6007,41 +6252,710 @@
       <c r="R136" s="1"/>
       <c r="S136" s="1"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="E137" s="26"/>
+    <row r="137" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="83"/>
+      <c r="B137" s="54"/>
+      <c r="C137" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="D137" s="88">
+        <v>1</v>
+      </c>
+      <c r="E137" s="88">
+        <v>0.75</v>
+      </c>
+      <c r="F137" s="6">
+        <v>9</v>
+      </c>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="M137" s="1"/>
+      <c r="N137" s="1"/>
+      <c r="O137" s="1"/>
+      <c r="P137" s="1"/>
+      <c r="Q137" s="1"/>
+      <c r="R137" s="1"/>
+      <c r="S137" s="1"/>
+    </row>
+    <row r="138" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="84"/>
+      <c r="B138" s="55"/>
+      <c r="C138" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="D138" s="88">
+        <v>1</v>
+      </c>
+      <c r="E138" s="88">
+        <v>1</v>
+      </c>
+      <c r="F138" s="6">
+        <v>9</v>
+      </c>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
+      <c r="Q138" s="1"/>
+      <c r="R138" s="1"/>
+      <c r="S138" s="1"/>
+    </row>
+    <row r="139" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="B139" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C139" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="D139" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E139" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F139" s="6">
+        <v>9</v>
+      </c>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+    </row>
+    <row r="140" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="83"/>
+      <c r="B140" s="54"/>
+      <c r="C140" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="D140" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E140" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F140" s="6">
+        <v>9</v>
+      </c>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
+      <c r="Q140" s="1"/>
+      <c r="R140" s="1"/>
+      <c r="S140" s="1"/>
+    </row>
+    <row r="141" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="83"/>
+      <c r="B141" s="54"/>
+      <c r="C141" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="D141" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E141" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F141" s="6">
+        <v>9</v>
+      </c>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
+      <c r="O141" s="1"/>
+      <c r="P141" s="1"/>
+      <c r="Q141" s="1"/>
+      <c r="R141" s="1"/>
+      <c r="S141" s="1"/>
+    </row>
+    <row r="142" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="83"/>
+      <c r="B142" s="54"/>
+      <c r="C142" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="D142" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="E142" s="88">
+        <v>2</v>
+      </c>
+      <c r="F142" s="6">
+        <v>9</v>
+      </c>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
+      <c r="Q142" s="1"/>
+      <c r="R142" s="1"/>
+      <c r="S142" s="1"/>
+    </row>
+    <row r="143" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="83"/>
+      <c r="B143" s="54"/>
+      <c r="C143" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="D143" s="88">
+        <v>2.5</v>
+      </c>
+      <c r="E143" s="88">
+        <v>2.25</v>
+      </c>
+      <c r="F143" s="6">
+        <v>9</v>
+      </c>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
+      <c r="Q143" s="1"/>
+      <c r="R143" s="1"/>
+      <c r="S143" s="1"/>
+    </row>
+    <row r="144" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="83"/>
+      <c r="B144" s="54"/>
+      <c r="C144" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="D144" s="88">
+        <v>2</v>
+      </c>
+      <c r="E144" s="88">
+        <v>2</v>
+      </c>
+      <c r="F144" s="6">
+        <v>9</v>
+      </c>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
+      <c r="Q144" s="1"/>
+      <c r="R144" s="1"/>
+      <c r="S144" s="1"/>
+    </row>
+    <row r="145" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="83"/>
+      <c r="B145" s="54"/>
+      <c r="C145" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D145" s="88">
+        <v>1.5</v>
+      </c>
+      <c r="E145" s="88">
+        <v>2</v>
+      </c>
+      <c r="F145" s="6">
+        <v>9</v>
+      </c>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="M145" s="1"/>
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="1"/>
+      <c r="S145" s="1"/>
+    </row>
+    <row r="146" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="83"/>
+      <c r="B146" s="55"/>
+      <c r="C146" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="D146" s="88">
+        <v>2</v>
+      </c>
+      <c r="E146" s="88">
+        <v>2.5</v>
+      </c>
+      <c r="F146" s="6">
+        <v>9</v>
+      </c>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1"/>
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+      <c r="Q146" s="1"/>
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+    </row>
+    <row r="147" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="B147" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C147" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D147" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E147" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F147" s="6">
+        <v>9</v>
+      </c>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+      <c r="L147" s="1"/>
+      <c r="M147" s="1"/>
+      <c r="N147" s="1"/>
+      <c r="O147" s="1"/>
+      <c r="P147" s="1"/>
+      <c r="Q147" s="1"/>
+      <c r="R147" s="1"/>
+      <c r="S147" s="1"/>
+    </row>
+    <row r="148" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="83"/>
+      <c r="B148" s="54"/>
+      <c r="C148" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D148" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E148" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F148" s="6">
+        <v>9</v>
+      </c>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="M148" s="1"/>
+      <c r="N148" s="1"/>
+      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
+      <c r="Q148" s="1"/>
+      <c r="R148" s="1"/>
+      <c r="S148" s="1"/>
+    </row>
+    <row r="149" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="83"/>
+      <c r="B149" s="54"/>
+      <c r="C149" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D149" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E149" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F149" s="6">
+        <v>9</v>
+      </c>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+      <c r="L149" s="1"/>
+      <c r="M149" s="1"/>
+      <c r="N149" s="1"/>
+      <c r="O149" s="1"/>
+      <c r="P149" s="1"/>
+      <c r="Q149" s="1"/>
+      <c r="R149" s="1"/>
+      <c r="S149" s="1"/>
+    </row>
+    <row r="150" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="83"/>
+      <c r="B150" s="55"/>
+      <c r="C150" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="D150" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="E150" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="F150" s="6">
+        <v>9</v>
+      </c>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+      <c r="Q150" s="1"/>
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+    </row>
+    <row r="151" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="78"/>
+      <c r="B151" s="45"/>
+      <c r="C151" s="39"/>
+      <c r="D151" s="35"/>
+      <c r="E151" s="35"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+    </row>
+    <row r="152" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A152" s="48"/>
+      <c r="B152" s="49"/>
+      <c r="C152" s="39"/>
+      <c r="D152" s="35"/>
+      <c r="E152" s="35"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="N152" s="1"/>
+      <c r="O152" s="1"/>
+      <c r="P152" s="1"/>
+      <c r="Q152" s="1"/>
+      <c r="R152" s="1"/>
+      <c r="S152" s="1"/>
+    </row>
+    <row r="153" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A153" s="48"/>
+      <c r="B153" s="37"/>
+      <c r="C153" s="39"/>
+      <c r="D153" s="35"/>
+      <c r="E153" s="35"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="M153" s="1"/>
+      <c r="N153" s="1"/>
+      <c r="O153" s="1"/>
+      <c r="P153" s="1"/>
+      <c r="Q153" s="1"/>
+      <c r="R153" s="1"/>
+      <c r="S153" s="1"/>
+    </row>
+    <row r="154" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A154" s="48"/>
+      <c r="B154" s="37"/>
+      <c r="C154" s="39"/>
+      <c r="D154" s="35"/>
+      <c r="E154" s="35"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1"/>
+      <c r="N154" s="1"/>
+      <c r="O154" s="1"/>
+      <c r="P154" s="1"/>
+      <c r="Q154" s="1"/>
+      <c r="R154" s="1"/>
+      <c r="S154" s="1"/>
+    </row>
+    <row r="155" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="45"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="28"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="M155" s="1"/>
+      <c r="N155" s="1"/>
+      <c r="O155" s="1"/>
+      <c r="P155" s="1"/>
+      <c r="Q155" s="1"/>
+      <c r="R155" s="1"/>
+      <c r="S155" s="1"/>
+    </row>
+    <row r="156" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A156" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B156" s="3"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="36"/>
+      <c r="E156" s="8"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
+      <c r="Q156" s="1"/>
+      <c r="R156" s="1"/>
+      <c r="S156" s="1"/>
+    </row>
+    <row r="157" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A157" s="7"/>
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+      <c r="N157" s="1"/>
+      <c r="O157" s="1"/>
+      <c r="P157" s="1"/>
+      <c r="Q157" s="1"/>
+      <c r="R157" s="1"/>
+      <c r="S157" s="1"/>
+    </row>
+    <row r="158" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="5"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="M158" s="1"/>
+      <c r="N158" s="1"/>
+      <c r="O158" s="1"/>
+      <c r="P158" s="1"/>
+      <c r="Q158" s="1"/>
+      <c r="R158" s="1"/>
+      <c r="S158" s="1"/>
+    </row>
+    <row r="159" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A159" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B159" s="3"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="8"/>
+      <c r="E159" s="8"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
+      <c r="O159" s="1"/>
+      <c r="P159" s="1"/>
+      <c r="Q159" s="1"/>
+      <c r="R159" s="1"/>
+      <c r="S159" s="1"/>
+    </row>
+    <row r="160" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
+      <c r="O160" s="1"/>
+      <c r="P160" s="1"/>
+      <c r="Q160" s="1"/>
+      <c r="R160" s="1"/>
+      <c r="S160" s="1"/>
+    </row>
+    <row r="161" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+      <c r="O161" s="1"/>
+      <c r="P161" s="1"/>
+      <c r="Q161" s="1"/>
+      <c r="R161" s="1"/>
+      <c r="S161" s="1"/>
+    </row>
+    <row r="162" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A162" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B162" s="4"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="11">
+        <f>SUM(D4:D161)</f>
+        <v>317.39999999999975</v>
+      </c>
+      <c r="E162" s="11">
+        <f>SUM(E4:E161)</f>
+        <v>316.72999999999996</v>
+      </c>
+      <c r="F162" s="6"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+      <c r="L162" s="1"/>
+      <c r="M162" s="1"/>
+      <c r="N162" s="1"/>
+      <c r="O162" s="1"/>
+      <c r="P162" s="1"/>
+      <c r="Q162" s="1"/>
+      <c r="R162" s="1"/>
+      <c r="S162" s="1"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E163" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="A84:A113"/>
-    <mergeCell ref="B84:B113"/>
-    <mergeCell ref="A114:A116"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A69"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
+  <mergeCells count="61">
+    <mergeCell ref="B121:B125"/>
+    <mergeCell ref="B126:B131"/>
+    <mergeCell ref="B132:B138"/>
+    <mergeCell ref="B139:B146"/>
+    <mergeCell ref="B147:B150"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A126:A131"/>
+    <mergeCell ref="A132:A138"/>
+    <mergeCell ref="A139:A146"/>
+    <mergeCell ref="A147:A150"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="B8:B14"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B19:B20"/>
@@ -6052,17 +6966,36 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="B8:B14"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="A84:A113"/>
+    <mergeCell ref="B84:B113"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B117:B120"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -6327,11 +7260,11 @@
       </c>
       <c r="K6" s="18">
         <f t="shared" si="1"/>
-        <v>226.51999999999998</v>
+        <v>183.26999999999998</v>
       </c>
       <c r="L6" s="18">
         <f t="shared" si="1"/>
-        <v>226.51999999999998</v>
+        <v>183.26999999999998</v>
       </c>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
@@ -6445,7 +7378,7 @@
       </c>
       <c r="K9" s="18">
         <f>SUMIF('Product Backlog'!F:F,9,'Product Backlog'!E:E)</f>
-        <v>0</v>
+        <v>43.25</v>
       </c>
       <c r="L9" s="18">
         <f>SUMIF('Product Backlog'!F:F,10,'Product Backlog'!E:E)</f>
@@ -6453,11 +7386,11 @@
       </c>
       <c r="M9" s="18">
         <f>SUM(C9:L9)</f>
-        <v>273.48</v>
+        <v>316.73</v>
       </c>
       <c r="N9" s="18">
         <f>M9/10</f>
-        <v>27.348000000000003</v>
+        <v>31.673000000000002</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -6472,11 +7405,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -6489,6 +7417,11 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>